<commit_message>
pushing before fixing concat index error
</commit_message>
<xml_diff>
--- a/mean_results/avg_train_results_80_20.xlsx
+++ b/mean_results/avg_train_results_80_20.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,7 +489,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>RandomForestClassifier</t>
+          <t>RandomForestClassifier-train</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -602,13 +602,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.6697165476779529</v>
+        <v>0.624234693877551</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7526315789473684</v>
+        <v>0.7631578947368421</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7082702083682475</v>
+        <v>0.6861287008499113</v>
       </c>
       <c r="F7" t="n">
         <v>38</v>
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.8126239122392189</v>
+        <v>0.8056327985739751</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7418181818181818</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7751919360848933</v>
+        <v>0.7368850697856011</v>
       </c>
       <c r="F8" t="n">
         <v>55</v>
@@ -642,16 +642,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.746236559139785</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="D9" t="n">
-        <v>0.746236559139785</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="E9" t="n">
-        <v>0.746236559139785</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="F9" t="n">
-        <v>0.746236559139785</v>
+        <v>0.7139784946236559</v>
       </c>
     </row>
     <row r="10">
@@ -662,13 +662,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.7411702299585859</v>
+        <v>0.714933746225763</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7472248803827751</v>
+        <v>0.7215789473684211</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7417310722265704</v>
+        <v>0.7115068853177562</v>
       </c>
       <c r="F10" t="n">
         <v>93</v>
@@ -682,13 +682,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.7542316557518198</v>
+        <v>0.7315131428915652</v>
       </c>
       <c r="D11" t="n">
-        <v>0.746236559139785</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7478475742221778</v>
+        <v>0.7161459082849966</v>
       </c>
       <c r="F11" t="n">
         <v>93</v>
@@ -697,7 +697,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>DecisionTreeClassifier</t>
+          <t>LGBMClassifier-train</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
@@ -706,13 +706,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6459637771946337</v>
+        <v>0.624234693877551</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7315789473684211</v>
+        <v>0.7631578947368421</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6832862877438892</v>
+        <v>0.6861287008499113</v>
       </c>
       <c r="F12" t="n">
         <v>38</v>
@@ -726,13 +726,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.7989686657609282</v>
+        <v>0.8056327985739751</v>
       </c>
       <c r="D13" t="n">
-        <v>0.72</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>0.755029490399759</v>
+        <v>0.7368850697856011</v>
       </c>
       <c r="F13" t="n">
         <v>55</v>
@@ -746,16 +746,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.724731182795699</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="D14" t="n">
-        <v>0.724731182795699</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="E14" t="n">
-        <v>0.724731182795699</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="F14" t="n">
-        <v>0.724731182795699</v>
+        <v>0.7139784946236559</v>
       </c>
     </row>
     <row r="15">
@@ -766,13 +766,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.7224662214777809</v>
+        <v>0.714933746225763</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7257894736842105</v>
+        <v>0.7215789473684211</v>
       </c>
       <c r="E15" t="n">
-        <v>0.7191578890718241</v>
+        <v>0.7115068853177562</v>
       </c>
       <c r="F15" t="n">
         <v>93</v>
@@ -786,13 +786,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.7364505392499692</v>
+        <v>0.7315131428915652</v>
       </c>
       <c r="D16" t="n">
-        <v>0.724731182795699</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="E16" t="n">
-        <v>0.7257150635081133</v>
+        <v>0.7161459082849966</v>
       </c>
       <c r="F16" t="n">
         <v>93</v>
@@ -801,7 +801,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>SVC</t>
+          <t>DecisionTreeClassifier-train</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
@@ -810,13 +810,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.5862637362637362</v>
+        <v>0.6305200121910033</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6263157894736843</v>
+        <v>0.7157894736842105</v>
       </c>
       <c r="E17" t="n">
-        <v>0.5976140754222946</v>
+        <v>0.6608354282933878</v>
       </c>
       <c r="F17" t="n">
         <v>38</v>
@@ -830,13 +830,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.7269614914656729</v>
+        <v>0.7795171268061294</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.6836363636363636</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6968633235004915</v>
+        <v>0.7186122629926104</v>
       </c>
       <c r="F18" t="n">
         <v>55</v>
@@ -850,16 +850,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.6580645161290322</v>
+        <v>0.6967741935483871</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6580645161290322</v>
+        <v>0.6967741935483871</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6580645161290322</v>
+        <v>0.6967741935483871</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6580645161290322</v>
+        <v>0.6967741935483871</v>
       </c>
     </row>
     <row r="20">
@@ -870,13 +870,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.6566126138647046</v>
+        <v>0.7050185694985664</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6531578947368422</v>
+        <v>0.6997129186602871</v>
       </c>
       <c r="E20" t="n">
-        <v>0.6472386994613931</v>
+        <v>0.689723845642999</v>
       </c>
       <c r="F20" t="n">
         <v>93</v>
@@ -890,13 +890,13 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.6694720861143439</v>
+        <v>0.7186365853504865</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6580645161290322</v>
+        <v>0.6967741935483871</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6563098672964971</v>
+        <v>0.6950045240832506</v>
       </c>
       <c r="F21" t="n">
         <v>93</v>
@@ -905,7 +905,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>ElasticNet</t>
+          <t>ElasticNet-train</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
@@ -914,13 +914,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.5639402288012612</v>
+        <v>0.6027958781890327</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6263157894736843</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="E22" t="n">
-        <v>0.593381130435777</v>
+        <v>0.6401935319582379</v>
       </c>
       <c r="F22" t="n">
         <v>38</v>
@@ -934,13 +934,13 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.720652199341275</v>
+        <v>0.7595809173705457</v>
       </c>
       <c r="D23" t="n">
-        <v>0.6654545454545454</v>
+        <v>0.6872727272727273</v>
       </c>
       <c r="E23" t="n">
-        <v>0.6918625511325212</v>
+        <v>0.7209966002658774</v>
       </c>
       <c r="F23" t="n">
         <v>55</v>
@@ -954,16 +954,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.6494623655913978</v>
+        <v>0.6860215053763441</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6494623655913978</v>
+        <v>0.6860215053763441</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6494623655913978</v>
+        <v>0.6860215053763441</v>
       </c>
       <c r="F24" t="n">
-        <v>0.6494623655913978</v>
+        <v>0.6860215053763441</v>
       </c>
     </row>
     <row r="25">
@@ -974,13 +974,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.642296214071268</v>
+        <v>0.6811883977797892</v>
       </c>
       <c r="D25" t="n">
-        <v>0.6458851674641148</v>
+        <v>0.6857416267942584</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6426218407841491</v>
+        <v>0.6805950661120577</v>
       </c>
       <c r="F25" t="n">
         <v>93</v>
@@ -994,13 +994,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.6566193511636349</v>
+        <v>0.6955182131888522</v>
       </c>
       <c r="D26" t="n">
-        <v>0.6494623655913978</v>
+        <v>0.6860215053763441</v>
       </c>
       <c r="E26" t="n">
-        <v>0.65162283084783</v>
+        <v>0.6879802927853366</v>
       </c>
       <c r="F26" t="n">
         <v>93</v>
@@ -1009,7 +1009,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>MLPClassifier</t>
+          <t>SVC-train</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
@@ -1018,13 +1018,13 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.325</v>
+        <v>0.5862637362637362</v>
       </c>
       <c r="D27" t="n">
-        <v>0.04736842105263155</v>
+        <v>0.6263157894736843</v>
       </c>
       <c r="E27" t="n">
-        <v>0.08157349896480333</v>
+        <v>0.5976140754222946</v>
       </c>
       <c r="F27" t="n">
         <v>38</v>
@@ -1038,13 +1038,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.6007871564718675</v>
+        <v>0.7269614914656729</v>
       </c>
       <c r="D28" t="n">
-        <v>0.989090909090909</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7472951522951524</v>
+        <v>0.6968633235004915</v>
       </c>
       <c r="F28" t="n">
         <v>55</v>
@@ -1058,16 +1058,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.6043010752688172</v>
+        <v>0.6580645161290322</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6043010752688172</v>
+        <v>0.6580645161290322</v>
       </c>
       <c r="E29" t="n">
-        <v>0.6043010752688172</v>
+        <v>0.6580645161290322</v>
       </c>
       <c r="F29" t="n">
-        <v>0.6043010752688172</v>
+        <v>0.6580645161290322</v>
       </c>
     </row>
     <row r="30">
@@ -1078,13 +1078,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.4628935782359337</v>
+        <v>0.6566126138647046</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5182296650717703</v>
+        <v>0.6531578947368422</v>
       </c>
       <c r="E30" t="n">
-        <v>0.4144343256299779</v>
+        <v>0.6472386994613931</v>
       </c>
       <c r="F30" t="n">
         <v>93</v>
@@ -1098,26 +1098,341 @@
         </is>
       </c>
       <c r="C31" t="n">
+        <v>0.6694720861143439</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.6580645161290322</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.6563098672964971</v>
+      </c>
+      <c r="F31" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>NeuralNetClassifier-train</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0.6669549175602445</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.631578947368421</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.5653703891794899</v>
+      </c>
+      <c r="F32" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n"/>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0.7627220653327725</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.6981818181818181</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.7097933436549082</v>
+      </c>
+      <c r="F33" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n"/>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0.6709677419354839</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.6709677419354839</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.6709677419354839</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.6709677419354839</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n"/>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>macro avg</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.7148384914465085</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.6648803827751196</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.6375818664171991</v>
+      </c>
+      <c r="F35" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n"/>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>weighted avg</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0.7235914028020621</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.6709677419354839</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.6507818138692534</v>
+      </c>
+      <c r="F36" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>NeuralNetClassifier</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0.6034722222222222</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.2631578947368421</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.3416402116402116</v>
+      </c>
+      <c r="F37" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n"/>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0.6338064793927752</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.8690909090909091</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.7303986817779922</v>
+      </c>
+      <c r="F38" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n"/>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0.621505376344086</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.621505376344086</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.621505376344086</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.621505376344086</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n"/>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>macro avg</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0.6186393508074988</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.5661244019138756</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.5360194467091018</v>
+      </c>
+      <c r="F40" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n"/>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>weighted avg</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>0.6214118366779255</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.621505376344086</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.5715511348399743</v>
+      </c>
+      <c r="F41" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>MLPClassifier-train</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>Did not Play: 0</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.04736842105263155</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.08157349896480333</v>
+      </c>
+      <c r="F42" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n"/>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>Played in the NHL: 1</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.6007871564718675</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.989090909090909</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.7472951522951524</v>
+      </c>
+      <c r="F43" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n"/>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0.6043010752688172</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.6043010752688172</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.6043010752688172</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.6043010752688172</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n"/>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>macro avg</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0.4628935782359337</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.5182296650717703</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.4144343256299779</v>
+      </c>
+      <c r="F45" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n"/>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>weighted avg</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
         <v>0.4880999312468034</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D46" t="n">
         <v>0.6043010752688172</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E46" t="n">
         <v>0.4752798530849021</v>
       </c>
-      <c r="F31" t="n">
+      <c r="F46" t="n">
         <v>93</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A42:A46"/>
     <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A32:A36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
pushing final from VS to server
</commit_message>
<xml_diff>
--- a/mean_results/avg_train_results_80_20.xlsx
+++ b/mean_results/avg_train_results_80_20.xlsx
@@ -1528,16 +1528,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A12:A16"/>
     <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A41"/>
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A32:A36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>